<commit_message>
Improved custom MIP code and added fancy plot codes to generate plots. Saved plots in Results
</commit_message>
<xml_diff>
--- a/Results/Simulation Results.xlsx
+++ b/Results/Simulation Results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TUM\Master Thesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TUM\Master-Thesis\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB4E739C-0952-4711-90BD-63D4D87D5A1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35136DFF-E1BC-4F21-98BA-067DEF9FE487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1935" yWindow="7620" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32355" yWindow="3330" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1359,8 +1359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{446446E8-E5A3-40A8-BFDE-ADF510F04626}">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1805,11 +1805,21 @@
       <c r="C12" s="4">
         <v>6</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="D12" s="2">
+        <v>0.91600000000000004</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.57399999999999995</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.34200000000000003</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="H12" s="2">
+        <v>63.77</v>
+      </c>
       <c r="J12" s="2">
         <v>100</v>
       </c>

</xml_diff>

<commit_message>
Revert "Mod selection measure"
</commit_message>
<xml_diff>
--- a/Results/Simulation Results.xlsx
+++ b/Results/Simulation Results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TUM\Master-Thesis\Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TUM\Master Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35136DFF-E1BC-4F21-98BA-067DEF9FE487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB4E739C-0952-4711-90BD-63D4D87D5A1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32355" yWindow="3330" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1935" yWindow="7620" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1359,8 +1359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{446446E8-E5A3-40A8-BFDE-ADF510F04626}">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1805,21 +1805,11 @@
       <c r="C12" s="4">
         <v>6</v>
       </c>
-      <c r="D12" s="2">
-        <v>0.91600000000000004</v>
-      </c>
-      <c r="E12" s="2">
-        <v>0.57399999999999995</v>
-      </c>
-      <c r="F12" s="2">
-        <v>0.34200000000000003</v>
-      </c>
-      <c r="G12" s="2">
-        <v>0.48499999999999999</v>
-      </c>
-      <c r="H12" s="2">
-        <v>63.77</v>
-      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
       <c r="J12" s="2">
         <v>100</v>
       </c>

</xml_diff>